<commit_message>
actualização modelo pauta com visto e resolv. erro ao inserir nota por codigo de barra 5-dic-2017
</commit_message>
<xml_diff>
--- a/application/libraries/Modelos/Pauta_Modelo_Anual.xlsx
+++ b/application/libraries/Modelos/Pauta_Modelo_Anual.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="993"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="1º até 4º" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="145">
   <si>
     <t>Nº</t>
   </si>
@@ -453,13 +453,20 @@
   </si>
   <si>
     <t>120</t>
+  </si>
+  <si>
+    <t>Visto 
+Director Geral Adjunto para Área Académica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chefe de Departamento: </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -468,13 +475,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Arial Unicode MS"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
@@ -506,7 +506,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -566,11 +566,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -578,9 +666,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -602,9 +690,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -617,18 +702,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1053,7 +1176,7 @@
   <dimension ref="A2:L135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H131" sqref="H131:L131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1070,80 +1193,82 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-    </row>
-    <row r="3" spans="1:12" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
+      <c r="A2" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+    </row>
+    <row r="3" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
     </row>
     <row r="4" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-    </row>
-    <row r="5" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
+      <c r="A4" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="26"/>
+    </row>
+    <row r="5" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="31"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="29"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="33"/>
       <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -1153,15 +1278,15 @@
       <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="19"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="16"/>
+      <c r="J7" s="15"/>
       <c r="K7" s="4"/>
       <c r="L7" s="13"/>
     </row>
@@ -1173,15 +1298,15 @@
       <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="16"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
     </row>
@@ -5679,19 +5804,21 @@
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A131" s="2"/>
-      <c r="B131" s="21" t="s">
+      <c r="B131" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C131" s="22"/>
-      <c r="D131" s="22"/>
-      <c r="E131" s="22"/>
-      <c r="F131" s="22"/>
-      <c r="G131" s="22"/>
-      <c r="H131" s="22"/>
-      <c r="I131" s="22"/>
-      <c r="J131" s="22"/>
-      <c r="K131" s="23"/>
-      <c r="L131" s="2"/>
+      <c r="C131" s="21"/>
+      <c r="D131" s="21"/>
+      <c r="E131" s="21"/>
+      <c r="F131" s="21"/>
+      <c r="G131" s="36"/>
+      <c r="H131" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="I131" s="21"/>
+      <c r="J131" s="21"/>
+      <c r="K131" s="21"/>
+      <c r="L131" s="22"/>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A132" s="2"/>
@@ -5738,31 +5865,33 @@
     <row r="135" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
-      <c r="C135" s="20" t="s">
+      <c r="C135" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D135" s="20"/>
-      <c r="E135" s="20"/>
-      <c r="F135" s="20"/>
-      <c r="G135" s="20"/>
-      <c r="H135" s="20"/>
-      <c r="I135" s="20"/>
+      <c r="D135" s="19"/>
+      <c r="E135" s="19"/>
+      <c r="F135" s="19"/>
+      <c r="G135" s="19"/>
+      <c r="H135" s="19"/>
+      <c r="I135" s="19"/>
       <c r="J135" s="3"/>
       <c r="K135" s="2"/>
       <c r="L135" s="2"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="9">
+  <mergeCells count="11">
     <mergeCell ref="A2:L3"/>
     <mergeCell ref="D6:L6"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="C135:I135"/>
-    <mergeCell ref="B131:K131"/>
-    <mergeCell ref="A4:L5"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
+    <mergeCell ref="A4:B5"/>
+    <mergeCell ref="C4:L5"/>
+    <mergeCell ref="B131:F131"/>
+    <mergeCell ref="H131:L131"/>
   </mergeCells>
   <conditionalFormatting sqref="L10:L129">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Reprovado">

</xml_diff>